<commit_message>
HOJA2(excel) SE AGREGAN FORMATOS DE ARCHIVOS Y DESCRIPCIONES
</commit_message>
<xml_diff>
--- a/ANALISIS  DEL PROBLEMA/horario y materiras.xlsx
+++ b/ANALISIS  DEL PROBLEMA/horario y materiras.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\INFO II\TEORIA\PARCIAL 1 - ANDRES RIVERA\ANALISIS  DEL PROBLEMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D73C5E2-E38B-44F3-80EE-DC2313B0ED31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BB7237-6D05-4876-B8A8-ED6802DD0FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CURSOS Y HORARIO CLASES" sheetId="1" r:id="rId1"/>
-    <sheet name="SOLUCION A ED en tiempo RUN" sheetId="2" r:id="rId2"/>
+    <sheet name="SLN A LA DATA en tiempo RUN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -183,9 +183,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Sugerencia datos de estudio</t>
-  </si>
-  <si>
     <t>Para dar solucion a esto, se hará uso de una matriz de Nx7, donde N seran las horas y las columnas representan los días, para validar así lo espacios disponibles y porterior a ello dar una sugerencia acorde a lo necesitado</t>
   </si>
   <si>
@@ -201,23 +198,178 @@
     <t>D7</t>
   </si>
   <si>
-    <t>hora1</t>
-  </si>
-  <si>
-    <t>hora2</t>
-  </si>
-  <si>
-    <t>hora3</t>
-  </si>
-  <si>
-    <t>hora24</t>
+    <t>FORMATO DE TEXTO PARA INFO DE LOS CURSOS</t>
+  </si>
+  <si>
+    <t>FORMATO - HORARIO DE CLASE ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>FORMATO PARA USUARIOS</t>
+  </si>
+  <si>
+    <t>SUGERENCIA DATOS DE ESTUDIO</t>
+  </si>
+  <si>
+    <t>HORAS</t>
+  </si>
+  <si>
+    <t>00-24</t>
+  </si>
+  <si>
+    <t>00: Hora inicial Clase - 24: Hora Final Clase</t>
+  </si>
+  <si>
+    <t>diaN</t>
+  </si>
+  <si>
+    <t>Va despues del "punto y coma" y de tamaño maximo de 8 caracteres</t>
+  </si>
+  <si>
+    <t>CLAVE:</t>
+  </si>
+  <si>
+    <t>USUARIO:</t>
+  </si>
+  <si>
+    <t>Se deja como adminstrador al usuario master para gestionar los cursos, los demás usuarios seran estudiantes</t>
+  </si>
+  <si>
+    <t>PENDIENTE:</t>
+  </si>
+  <si>
+    <t>CUADRAR HORAS DE SUEÑO Y ALIMENTACIÓN</t>
+  </si>
+  <si>
+    <t>HORA</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN:</t>
+  </si>
+  <si>
+    <t>CURSOS</t>
+  </si>
+  <si>
+    <t>cursoN</t>
+  </si>
+  <si>
+    <t>Tope máximo 3 dias, otras solo toman 2; y su representación será por: LMWJVS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La celda(posición del arreglo) se rellenara con la respectivo ID  del curso correspondiente  a su horario, al igual que sus actividaes cotidianas como horas de sueño y alimentación. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nota: el arreglo estará inicializado con el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valor nulo (\0)</t>
+    </r>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMBIO1 </t>
+  </si>
+  <si>
+    <t>CAMBIO 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(13/14-04-2023)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción de como se manejará la información en la matriz que ayuadara a gestionar horaios de estudio personal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(13/14-04-2023)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SE AGREGAN FORMATOS DE ARCHIVOS PARA EL CRONOGRAMA ESTUDIANTIL (HORARIO DE CLASE ESTUDIANTE y USAURIOS), para si poder guradar  la información en el archivo</t>
+    </r>
+  </si>
+  <si>
+    <t>(13/14-04-2023) Se agrega formato de texto parala informacion de cada curso correspondiente. A las cursos de un credito se les asignará un total de 5 horas semanales, las cuales se repartiran entre las HTD y HTP</t>
+  </si>
+  <si>
+    <t>CUADRAR HORAS DE SUEÑO Y ALIMENTACIÓN y dudas si agrega la contraseña al usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +387,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -348,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -379,14 +539,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,6 +593,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>178594</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>107157</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>549642</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>125967</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{682BBD4F-A573-4AA7-8E0B-E5641BC6224E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11656219" y="678657"/>
+          <a:ext cx="3419048" cy="1923810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>268627</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>122574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>511969</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>115104</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ED65D81-80F3-454F-A193-D8591DB68F8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11746252" y="3170574"/>
+          <a:ext cx="3291342" cy="3231030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>699633</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>128140</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF9E5DCC-5941-4757-BD1A-CFF1578A961A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17692687" y="4226719"/>
+          <a:ext cx="3628571" cy="3580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L111"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,6 +2710,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
     <mergeCell ref="A96:A99"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="A104:A107"/>
@@ -2399,26 +2746,6 @@
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A60:A63"/>
     <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2427,413 +2754,1350 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C3E2EB-B927-45CA-9B97-F8A6A5130907}">
-  <dimension ref="A2:O38"/>
+  <dimension ref="A1:AL70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="6" width="11.7109375" customWidth="1"/>
+    <col min="29" max="29" width="13" customWidth="1"/>
+    <col min="38" max="38" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL2" s="24"/>
+    </row>
+    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="H4" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="AL3" s="24"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="O4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="AL4" s="24"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="H5" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="H5" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="AL5" s="24"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="H6" t="s">
         <v>41</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="H6" t="s">
-        <v>42</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="AL6" s="24"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="AL7" s="24"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="AL8" s="24"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="AL9" s="24"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="AL10" s="24"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="AL11" s="24"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="AL12" s="24"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="AL13" s="24"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="AL14" s="24"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="AL15" s="24"/>
+    </row>
+    <row r="16" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="AL16" s="24"/>
+    </row>
+    <row r="17" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="AL17" s="24"/>
+    </row>
+    <row r="18" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL18" s="24"/>
+    </row>
+    <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="24"/>
+      <c r="AG19" s="24"/>
+      <c r="AH19" s="24"/>
+      <c r="AI19" s="24"/>
+      <c r="AJ19" s="24"/>
+      <c r="AK19" s="24"/>
+      <c r="AL19" s="24"/>
+    </row>
+    <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL20" s="24"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="H18" s="1" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="O21" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="W21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AL21" s="24"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="18"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
+      <c r="AL22" s="24"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="H23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="H19" s="1" t="s">
+      <c r="K23" s="14"/>
+      <c r="L23" s="15"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="W23" s="18"/>
+      <c r="X23" s="18"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
+      <c r="AL23" s="24"/>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="H24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="W24" s="18"/>
+      <c r="X24" s="18"/>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
+      <c r="AA24" s="18"/>
+      <c r="AL24" s="24"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="18"/>
+      <c r="AC25" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD25" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="18"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="18"/>
+      <c r="AL25" s="24"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+      <c r="AA26" s="18"/>
+      <c r="AL26" s="24"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+      <c r="AA27" s="18"/>
+      <c r="AC27" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD27" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
+      <c r="AG27" s="22"/>
+      <c r="AH27" s="22"/>
+      <c r="AI27" s="22"/>
+      <c r="AJ27" s="22"/>
+      <c r="AL27" s="24"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="W28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AC28" s="29"/>
+      <c r="AD28" s="22"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="22"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="22"/>
+      <c r="AL28" s="24"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="H29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AL29" s="24"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="H30" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="W30" s="18"/>
+      <c r="X30" s="18"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
+      <c r="AL30" s="24"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="W31" s="18"/>
+      <c r="X31" s="18"/>
+      <c r="Y31" s="18"/>
+      <c r="Z31" s="18"/>
+      <c r="AA31" s="18"/>
+      <c r="AC31" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD31" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE31" s="22"/>
+      <c r="AF31" s="22"/>
+      <c r="AG31" s="22"/>
+      <c r="AH31" s="22"/>
+      <c r="AI31" s="22"/>
+      <c r="AJ31" s="22"/>
+      <c r="AL31" s="24"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18"/>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="22"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="22"/>
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
+      <c r="AL32" s="24"/>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="W33" s="18"/>
+      <c r="X33" s="18"/>
+      <c r="Y33" s="18"/>
+      <c r="Z33" s="18"/>
+      <c r="AA33" s="18"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="22"/>
+      <c r="AG33" s="22"/>
+      <c r="AH33" s="22"/>
+      <c r="AI33" s="22"/>
+      <c r="AJ33" s="22"/>
+      <c r="AL33" s="24"/>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="W34" s="18"/>
+      <c r="X34" s="18"/>
+      <c r="Y34" s="18"/>
+      <c r="Z34" s="18"/>
+      <c r="AA34" s="18"/>
+      <c r="AL34" s="24"/>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="W35" s="18"/>
+      <c r="X35" s="18"/>
+      <c r="Y35" s="18"/>
+      <c r="Z35" s="18"/>
+      <c r="AA35" s="18"/>
+      <c r="AL35" s="24"/>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="W36" s="18"/>
+      <c r="X36" s="18"/>
+      <c r="Y36" s="18"/>
+      <c r="Z36" s="18"/>
+      <c r="AA36" s="18"/>
+      <c r="AL36" s="24"/>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="W37" s="18"/>
+      <c r="X37" s="18"/>
+      <c r="Y37" s="18"/>
+      <c r="Z37" s="18"/>
+      <c r="AA37" s="18"/>
+      <c r="AL37" s="24"/>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="W38" s="18"/>
+      <c r="X38" s="18"/>
+      <c r="Y38" s="18"/>
+      <c r="Z38" s="18"/>
+      <c r="AA38" s="18"/>
+      <c r="AL38" s="24"/>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="W39" s="18"/>
+      <c r="X39" s="18"/>
+      <c r="Y39" s="18"/>
+      <c r="Z39" s="18"/>
+      <c r="AA39" s="18"/>
+      <c r="AL39" s="24"/>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="W40" s="18"/>
+      <c r="X40" s="18"/>
+      <c r="Y40" s="18"/>
+      <c r="Z40" s="18"/>
+      <c r="AA40" s="18"/>
+      <c r="AL40" s="24"/>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="W41" s="18"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="18"/>
+      <c r="Z41" s="18"/>
+      <c r="AA41" s="18"/>
+      <c r="AL41" s="24"/>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="20"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="26"/>
+      <c r="AA42" s="26"/>
+      <c r="AL42" s="24"/>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="20"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="26"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="26"/>
+      <c r="AL43" s="24"/>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="20"/>
+      <c r="AL44" s="24"/>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="AL45" s="24"/>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="24"/>
+      <c r="Z46" s="24"/>
+      <c r="AA46" s="24"/>
+      <c r="AB46" s="24"/>
+      <c r="AC46" s="24"/>
+      <c r="AD46" s="24"/>
+      <c r="AE46" s="24"/>
+      <c r="AF46" s="24"/>
+      <c r="AG46" s="24"/>
+      <c r="AH46" s="24"/>
+      <c r="AI46" s="24"/>
+      <c r="AJ46" s="24"/>
+      <c r="AK46" s="24"/>
+      <c r="AL46" s="24"/>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="AL47" s="24"/>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="H48" t="s">
+        <v>70</v>
+      </c>
+      <c r="I48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J48" t="s">
+        <v>47</v>
+      </c>
+      <c r="K48" t="s">
+        <v>48</v>
+      </c>
+      <c r="L48" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="I31" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" t="s">
-        <v>47</v>
-      </c>
-      <c r="K31" t="s">
-        <v>48</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="M48" t="s">
         <v>53</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N48" t="s">
         <v>54</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O48" t="s">
         <v>55</v>
       </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="H32" t="s">
-        <v>57</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="H33" t="s">
-        <v>58</v>
-      </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="H34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="H35" t="s">
+      <c r="AL48" s="24"/>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="20"/>
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="AL49" s="24"/>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="Q50" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
+      <c r="T50" s="16"/>
+      <c r="U50" s="16"/>
+      <c r="AL50" s="24"/>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="H51">
+        <v>3</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="Q51" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="AL51" s="24"/>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="H52" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="H36" t="s">
-        <v>60</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+      <c r="T52" s="16"/>
+      <c r="U52" s="16"/>
+      <c r="AL52" s="24"/>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="H53">
+        <v>24</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="16"/>
+      <c r="AL53" s="24"/>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="16"/>
+      <c r="U54" s="16"/>
+      <c r="AL54" s="24"/>
+    </row>
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="16"/>
+      <c r="AL55" s="24"/>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="16"/>
+      <c r="AL56" s="24"/>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+      <c r="T57" s="16"/>
+      <c r="U57" s="16"/>
+      <c r="AL57" s="24"/>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+      <c r="T58" s="16"/>
+      <c r="U58" s="16"/>
+      <c r="AL58" s="24"/>
+    </row>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+      <c r="T59" s="16"/>
+      <c r="U59" s="16"/>
+      <c r="AL59" s="24"/>
+    </row>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q60" s="20"/>
+      <c r="AL60" s="24"/>
+    </row>
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL61" s="24"/>
+    </row>
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL62" s="24"/>
+    </row>
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="AL63" s="24"/>
+    </row>
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="27"/>
+      <c r="M64" s="27"/>
+      <c r="AL64" s="24"/>
+    </row>
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A65" s="19"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="27"/>
+      <c r="AL65" s="24"/>
+    </row>
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL66" s="24"/>
+    </row>
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL67" s="24"/>
+    </row>
+    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL68" s="24"/>
+    </row>
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL69" s="24"/>
+    </row>
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="24"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="24"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="24"/>
+      <c r="S70" s="24"/>
+      <c r="T70" s="24"/>
+      <c r="U70" s="24"/>
+      <c r="V70" s="24"/>
+      <c r="W70" s="24"/>
+      <c r="X70" s="24"/>
+      <c r="Y70" s="24"/>
+      <c r="Z70" s="24"/>
+      <c r="AA70" s="24"/>
+      <c r="AB70" s="24"/>
+      <c r="AC70" s="24"/>
+      <c r="AD70" s="24"/>
+      <c r="AE70" s="24"/>
+      <c r="AF70" s="24"/>
+      <c r="AG70" s="24"/>
+      <c r="AH70" s="24"/>
+      <c r="AI70" s="24"/>
+      <c r="AJ70" s="24"/>
+      <c r="AK70" s="24"/>
+      <c r="AL70" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="A29:A38"/>
-    <mergeCell ref="B29:F38"/>
-    <mergeCell ref="B2:F11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B16:F25"/>
-    <mergeCell ref="A16:A25"/>
+  <mergeCells count="34">
+    <mergeCell ref="A63:M63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:M65"/>
+    <mergeCell ref="AD31:AJ33"/>
+    <mergeCell ref="AC31:AC33"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:M44"/>
+    <mergeCell ref="A42:M42"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:M17"/>
+    <mergeCell ref="AD25:AJ25"/>
+    <mergeCell ref="AD27:AJ28"/>
+    <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="B48:F57"/>
+    <mergeCell ref="W21:AA21"/>
+    <mergeCell ref="W22:AA41"/>
+    <mergeCell ref="A48:A57"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="I35:M35"/>
+    <mergeCell ref="Q51:U59"/>
+    <mergeCell ref="Q50:U50"/>
+    <mergeCell ref="J30:M31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="O5:S15"/>
+    <mergeCell ref="O4:S4"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O22:S39"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="B3:F12"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B21:F30"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A15:M15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HOJA2(excel) SE AGREGA ESTRUCUTRA para LA DATA EN RUNTIME PARA CURSOS Y HORARIO
</commit_message>
<xml_diff>
--- a/ANALISIS  DEL PROBLEMA/horario y materiras.xlsx
+++ b/ANALISIS  DEL PROBLEMA/horario y materiras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\INFO II\TEORIA\PARCIAL 1 - ANDRES RIVERA\ANALISIS  DEL PROBLEMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BB7237-6D05-4876-B8A8-ED6802DD0FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012C21D9-E5A3-4BC2-8A43-662162E6AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>CUADRAR HORAS DE SUEÑO Y ALIMENTACIÓN y dudas si agrega la contraseña al usuario</t>
+  </si>
+  <si>
+    <t>MANEJO DE LA INFORMACIÓN CURSOS</t>
+  </si>
+  <si>
+    <t>MANEJO DE LA INFORMACIÓN HORARIO-ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>NOTA: si algo se tiene pensado en separar el nombre del curso en otro arreglo, de momento se va a amnejar de esta forma como se planteo.</t>
   </si>
 </sst>
 </file>
@@ -508,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -518,6 +527,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,6 +551,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,44 +584,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,6 +733,93 @@
         <a:xfrm>
           <a:off x="17692687" y="4226719"/>
           <a:ext cx="3628571" cy="3580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>726281</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>38948</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AAAD629-C304-43FB-8CA5-41FBAED76EA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30777656" y="4726781"/>
+          <a:ext cx="12266667" cy="1857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>65143</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03644D17-BECB-4620-8CE2-C824AC4EA547}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect b="22020"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30813375" y="940594"/>
+          <a:ext cx="12257143" cy="1500187"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1008,20 +1107,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1045,11 +1144,11 @@
       <c r="I3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1210,58 +1309,58 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="15">
         <v>0.25</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1276,7 +1375,7 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1289,7 +1388,7 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1302,7 +1401,7 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1315,7 +1414,7 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="15">
         <v>0.29166666666666669</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1330,7 +1429,7 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1343,7 +1442,7 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
@@ -1356,7 +1455,7 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
@@ -1369,7 +1468,7 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="15">
         <v>0.33333333333333331</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1392,7 +1491,7 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1413,7 +1512,7 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1434,7 +1533,7 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
@@ -1455,7 +1554,7 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="15">
         <v>0.375</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1478,7 +1577,7 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1499,7 +1598,7 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="1" t="s">
         <v>33</v>
       </c>
@@ -1520,7 +1619,7 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1541,7 +1640,7 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="15">
         <v>0.41666666666666702</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1556,7 +1655,7 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1569,7 +1668,7 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1582,7 +1681,7 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1595,7 +1694,7 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="15">
         <v>0.45833333333333298</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1610,7 +1709,7 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1623,7 +1722,7 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1" t="s">
         <v>33</v>
       </c>
@@ -1636,7 +1735,7 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1649,7 +1748,7 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="15">
         <v>0.5</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1664,7 +1763,7 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="1" t="s">
         <v>32</v>
       </c>
@@ -1677,7 +1776,7 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="1" t="s">
         <v>33</v>
       </c>
@@ -1690,7 +1789,7 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="1" t="s">
         <v>34</v>
       </c>
@@ -1703,7 +1802,7 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="A44" s="15">
         <v>0.54166666666666696</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1718,7 +1817,7 @@
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="1" t="s">
         <v>32</v>
       </c>
@@ -1731,7 +1830,7 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="1" t="s">
         <v>33</v>
       </c>
@@ -1744,7 +1843,7 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="1" t="s">
         <v>34</v>
       </c>
@@ -1757,7 +1856,7 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+      <c r="A48" s="15">
         <v>0.58333333333333304</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1778,7 +1877,7 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1" t="s">
         <v>32</v>
       </c>
@@ -1797,7 +1896,7 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="1" t="s">
         <v>33</v>
       </c>
@@ -1816,7 +1915,7 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="1" t="s">
         <v>34</v>
       </c>
@@ -1835,7 +1934,7 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="15">
         <v>0.625</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1856,7 +1955,7 @@
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="1" t="s">
         <v>32</v>
       </c>
@@ -1875,7 +1974,7 @@
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="1" t="s">
         <v>33</v>
       </c>
@@ -1894,7 +1993,7 @@
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="1" t="s">
         <v>34</v>
       </c>
@@ -1913,7 +2012,7 @@
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="15">
         <v>0.66666666666666696</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1930,7 +2029,7 @@
       <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="9"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
@@ -1945,7 +2044,7 @@
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="1" t="s">
         <v>33</v>
       </c>
@@ -1960,7 +2059,7 @@
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="1" t="s">
         <v>34</v>
       </c>
@@ -1975,7 +2074,7 @@
       <c r="I59" s="1"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="A60" s="15">
         <v>0.70833333333333404</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1994,7 +2093,7 @@
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="1" t="s">
         <v>32</v>
       </c>
@@ -2011,7 +2110,7 @@
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="1" t="s">
         <v>33</v>
       </c>
@@ -2028,7 +2127,7 @@
       <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="1" t="s">
         <v>34</v>
       </c>
@@ -2045,7 +2144,7 @@
       <c r="I63" s="1"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="A64" s="15">
         <v>0.75</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2064,7 +2163,7 @@
       <c r="I64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="9"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="1" t="s">
         <v>32</v>
       </c>
@@ -2081,7 +2180,7 @@
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="1" t="s">
         <v>33</v>
       </c>
@@ -2098,7 +2197,7 @@
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="1" t="s">
         <v>34</v>
       </c>
@@ -2115,7 +2214,7 @@
       <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="15">
         <v>0.79166666666666696</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2130,7 +2229,7 @@
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="1" t="s">
         <v>32</v>
       </c>
@@ -2143,7 +2242,7 @@
       <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="1" t="s">
         <v>33</v>
       </c>
@@ -2156,7 +2255,7 @@
       <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="1" t="s">
         <v>34</v>
       </c>
@@ -2169,7 +2268,7 @@
       <c r="I71" s="1"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+      <c r="A72" s="15">
         <v>0.83333333333333404</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2184,7 +2283,7 @@
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="1" t="s">
         <v>32</v>
       </c>
@@ -2197,7 +2296,7 @@
       <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="1" t="s">
         <v>33</v>
       </c>
@@ -2210,7 +2309,7 @@
       <c r="I74" s="1"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="1" t="s">
         <v>34</v>
       </c>
@@ -2223,7 +2322,7 @@
       <c r="I75" s="1"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+      <c r="A76" s="15">
         <v>0.875</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2238,7 +2337,7 @@
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="9"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="1" t="s">
         <v>32</v>
       </c>
@@ -2251,7 +2350,7 @@
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="1" t="s">
         <v>33</v>
       </c>
@@ -2264,7 +2363,7 @@
       <c r="I78" s="1"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="1" t="s">
         <v>34</v>
       </c>
@@ -2277,7 +2376,7 @@
       <c r="I79" s="1"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
+      <c r="A80" s="15">
         <v>0.91666666666666696</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -2292,7 +2391,7 @@
       <c r="I80" s="1"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="9"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="1" t="s">
         <v>32</v>
       </c>
@@ -2305,7 +2404,7 @@
       <c r="I81" s="1"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="1" t="s">
         <v>33</v>
       </c>
@@ -2318,7 +2417,7 @@
       <c r="I82" s="1"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="9"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="1" t="s">
         <v>34</v>
       </c>
@@ -2331,7 +2430,7 @@
       <c r="I83" s="1"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+      <c r="A84" s="15">
         <v>0.95833333333333404</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2346,7 +2445,7 @@
       <c r="I84" s="1"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="1" t="s">
         <v>32</v>
       </c>
@@ -2359,7 +2458,7 @@
       <c r="I85" s="1"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
+      <c r="A86" s="15"/>
       <c r="B86" s="1" t="s">
         <v>33</v>
       </c>
@@ -2372,7 +2471,7 @@
       <c r="I86" s="1"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="1" t="s">
         <v>34</v>
       </c>
@@ -2385,7 +2484,7 @@
       <c r="I87" s="1"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
+      <c r="A88" s="15">
         <v>1</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2400,7 +2499,7 @@
       <c r="I88" s="1"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="1" t="s">
         <v>32</v>
       </c>
@@ -2413,7 +2512,7 @@
       <c r="I89" s="1"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="1" t="s">
         <v>33</v>
       </c>
@@ -2426,7 +2525,7 @@
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="1" t="s">
         <v>34</v>
       </c>
@@ -2439,7 +2538,7 @@
       <c r="I91" s="1"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="9">
+      <c r="A92" s="15">
         <v>1.0416666666666701</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -2454,7 +2553,7 @@
       <c r="I92" s="1"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="1" t="s">
         <v>32</v>
       </c>
@@ -2467,7 +2566,7 @@
       <c r="I93" s="1"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
+      <c r="A94" s="15"/>
       <c r="B94" s="1" t="s">
         <v>33</v>
       </c>
@@ -2480,7 +2579,7 @@
       <c r="I94" s="1"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="9"/>
+      <c r="A95" s="15"/>
       <c r="B95" s="1" t="s">
         <v>34</v>
       </c>
@@ -2493,7 +2592,7 @@
       <c r="I95" s="1"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="9">
+      <c r="A96" s="15">
         <v>1.0833333333333399</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2508,7 +2607,7 @@
       <c r="I96" s="1"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="9"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="1" t="s">
         <v>32</v>
       </c>
@@ -2521,7 +2620,7 @@
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="1" t="s">
         <v>33</v>
       </c>
@@ -2534,7 +2633,7 @@
       <c r="I98" s="1"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="9"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="1" t="s">
         <v>34</v>
       </c>
@@ -2547,7 +2646,7 @@
       <c r="I99" s="1"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="9">
+      <c r="A100" s="15">
         <v>1.12500000000001</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -2562,7 +2661,7 @@
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="9"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="1" t="s">
         <v>32</v>
       </c>
@@ -2575,7 +2674,7 @@
       <c r="I101" s="1"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="1" t="s">
         <v>33</v>
       </c>
@@ -2588,7 +2687,7 @@
       <c r="I102" s="1"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="9"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="1" t="s">
         <v>34</v>
       </c>
@@ -2601,7 +2700,7 @@
       <c r="I103" s="1"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="9">
+      <c r="A104" s="15">
         <v>1.1666666666666801</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -2616,7 +2715,7 @@
       <c r="I104" s="1"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="9"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="1" t="s">
         <v>32</v>
       </c>
@@ -2629,7 +2728,7 @@
       <c r="I105" s="1"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="9"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="1" t="s">
         <v>33</v>
       </c>
@@ -2642,7 +2741,7 @@
       <c r="I106" s="1"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="9"/>
+      <c r="A107" s="15"/>
       <c r="B107" s="1" t="s">
         <v>34</v>
       </c>
@@ -2655,7 +2754,7 @@
       <c r="I107" s="1"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="9">
+      <c r="A108" s="15">
         <v>1.2083333333333499</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -2670,7 +2769,7 @@
       <c r="I108" s="1"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="9"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="1" t="s">
         <v>32</v>
       </c>
@@ -2683,7 +2782,7 @@
       <c r="I109" s="1"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="9"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="1" t="s">
         <v>33</v>
       </c>
@@ -2696,7 +2795,7 @@
       <c r="I110" s="1"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="9"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="1" t="s">
         <v>34</v>
       </c>
@@ -2710,26 +2809,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
     <mergeCell ref="A96:A99"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="A104:A107"/>
@@ -2746,6 +2825,26 @@
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A60:A63"/>
     <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2754,10 +2853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C3E2EB-B927-45CA-9B97-F8A6A5130907}">
-  <dimension ref="A1:AL70"/>
+  <dimension ref="A1:BD70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AK1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AS19" sqref="AS19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,69 +2867,87 @@
     <col min="38" max="38" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL2" s="24"/>
-    </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+    </row>
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AL2" s="12"/>
+    </row>
+    <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="AL3" s="24"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="AL3" s="12"/>
+      <c r="AO3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP3" s="31"/>
+      <c r="AQ3" s="31"/>
+      <c r="AR3" s="31"/>
+      <c r="AS3" s="31"/>
+      <c r="AT3" s="31"/>
+      <c r="AU3" s="31"/>
+      <c r="AV3" s="31"/>
+      <c r="AW3" s="31"/>
+      <c r="AX3" s="31"/>
+      <c r="AY3" s="31"/>
+      <c r="AZ3" s="31"/>
+      <c r="BA3" s="31"/>
+      <c r="BB3" s="31"/>
+      <c r="BC3" s="31"/>
+      <c r="BD3" s="31"/>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
       <c r="O4" s="19" t="s">
         <v>56</v>
       </c>
@@ -2838,15 +2955,15 @@
       <c r="Q4" s="19"/>
       <c r="R4" s="19"/>
       <c r="S4" s="19"/>
-      <c r="AL4" s="24"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="AL4" s="12"/>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
       <c r="H5" t="s">
         <v>40</v>
       </c>
@@ -2865,20 +2982,20 @@
       <c r="M5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="AL5" s="24"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="AL5" s="12"/>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
       <c r="H6" t="s">
         <v>41</v>
       </c>
@@ -2887,20 +3004,20 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="AL6" s="24"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="AL6" s="12"/>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
       <c r="H7" t="s">
         <v>42</v>
       </c>
@@ -2909,100 +3026,100 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="AL7" s="24"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="AL8" s="24"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="AL9" s="24"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="AL10" s="24"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="AL11" s="24"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="AL12" s="24"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="AL13" s="24"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="AL14" s="24"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="AL7" s="12"/>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="AL8" s="12"/>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="AL9" s="12"/>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="AL10" s="12"/>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="AL11" s="12"/>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="AL12" s="12"/>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="AL13" s="12"/>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="AL14" s="12"/>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>76</v>
       </c>
@@ -3018,106 +3135,109 @@
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="AL15" s="24"/>
-    </row>
-    <row r="16" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="AL15" s="12"/>
+    </row>
+    <row r="16" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="AL16" s="24"/>
-    </row>
-    <row r="17" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="AL16" s="12"/>
+      <c r="AO16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="AL17" s="24"/>
-    </row>
-    <row r="18" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AL18" s="24"/>
-    </row>
-    <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
-      <c r="AE19" s="24"/>
-      <c r="AF19" s="24"/>
-      <c r="AG19" s="24"/>
-      <c r="AH19" s="24"/>
-      <c r="AI19" s="24"/>
-      <c r="AJ19" s="24"/>
-      <c r="AK19" s="24"/>
-      <c r="AL19" s="24"/>
-    </row>
-    <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AL20" s="24"/>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="AL17" s="12"/>
+    </row>
+    <row r="18" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL18" s="12"/>
+    </row>
+    <row r="19" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="12"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+    </row>
+    <row r="20" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL20" s="12"/>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
       <c r="O21" s="19" t="s">
         <v>57</v>
       </c>
@@ -3132,64 +3252,82 @@
       <c r="Y21" s="19"/>
       <c r="Z21" s="19"/>
       <c r="AA21" s="19"/>
-      <c r="AL21" s="24"/>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AL22" s="24"/>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
+      <c r="AL21" s="12"/>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AL22" s="12"/>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
       <c r="H23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
-      <c r="AL23" s="24"/>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="24"/>
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="24"/>
+      <c r="AL23" s="12"/>
+      <c r="AO23" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP23" s="31"/>
+      <c r="AQ23" s="31"/>
+      <c r="AR23" s="31"/>
+      <c r="AS23" s="31"/>
+      <c r="AT23" s="31"/>
+      <c r="AU23" s="31"/>
+      <c r="AV23" s="31"/>
+      <c r="AW23" s="31"/>
+      <c r="AX23" s="31"/>
+      <c r="AY23" s="31"/>
+      <c r="AZ23" s="31"/>
+      <c r="BA23" s="31"/>
+      <c r="BB23" s="31"/>
+      <c r="BC23" s="31"/>
+      <c r="BD23" s="31"/>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
       <c r="H24" s="1" t="s">
         <v>50</v>
       </c>
@@ -3205,386 +3343,386 @@
       <c r="L24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="18"/>
-      <c r="AA24" s="18"/>
-      <c r="AL24" s="24"/>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="W25" s="18"/>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="18"/>
-      <c r="Z25" s="18"/>
-      <c r="AA25" s="18"/>
-      <c r="AC25" s="23" t="s">
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AL24" s="12"/>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="24"/>
+      <c r="AC25" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AD25" s="18" t="s">
+      <c r="AD25" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="AE25" s="18"/>
-      <c r="AF25" s="18"/>
-      <c r="AG25" s="18"/>
-      <c r="AH25" s="18"/>
-      <c r="AI25" s="18"/>
-      <c r="AJ25" s="18"/>
-      <c r="AL25" s="24"/>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="18"/>
-      <c r="AA26" s="18"/>
-      <c r="AL26" s="24"/>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="18"/>
-      <c r="Z27" s="18"/>
-      <c r="AA27" s="18"/>
-      <c r="AC27" s="29" t="s">
+      <c r="AE25" s="24"/>
+      <c r="AF25" s="24"/>
+      <c r="AG25" s="24"/>
+      <c r="AH25" s="24"/>
+      <c r="AI25" s="24"/>
+      <c r="AJ25" s="24"/>
+      <c r="AL25" s="12"/>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="24"/>
+      <c r="AL26" s="12"/>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="Z27" s="24"/>
+      <c r="AA27" s="24"/>
+      <c r="AC27" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AD27" s="22" t="s">
+      <c r="AD27" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
-      <c r="AG27" s="22"/>
-      <c r="AH27" s="22"/>
-      <c r="AI27" s="22"/>
-      <c r="AJ27" s="22"/>
-      <c r="AL27" s="24"/>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18"/>
-      <c r="Y28" s="18"/>
-      <c r="Z28" s="18"/>
-      <c r="AA28" s="18"/>
-      <c r="AC28" s="29"/>
-      <c r="AD28" s="22"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AL28" s="24"/>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="AE27" s="21"/>
+      <c r="AF27" s="21"/>
+      <c r="AG27" s="21"/>
+      <c r="AH27" s="21"/>
+      <c r="AI27" s="21"/>
+      <c r="AJ27" s="21"/>
+      <c r="AL27" s="12"/>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="24"/>
+      <c r="AC28" s="25"/>
+      <c r="AD28" s="21"/>
+      <c r="AE28" s="21"/>
+      <c r="AF28" s="21"/>
+      <c r="AG28" s="21"/>
+      <c r="AH28" s="21"/>
+      <c r="AI28" s="21"/>
+      <c r="AJ28" s="21"/>
+      <c r="AL28" s="12"/>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
       <c r="H29" t="s">
         <v>72</v>
       </c>
       <c r="I29" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="18"/>
-      <c r="Y29" s="18"/>
-      <c r="Z29" s="18"/>
-      <c r="AA29" s="18"/>
-      <c r="AL29" s="24"/>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="H30" s="22" t="s">
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="24"/>
+      <c r="Z29" s="24"/>
+      <c r="AA29" s="24"/>
+      <c r="AL29" s="12"/>
+    </row>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="H30" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="22" t="s">
+      <c r="I30" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="22" t="s">
+      <c r="J30" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18"/>
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="18"/>
-      <c r="AA30" s="18"/>
-      <c r="AL30" s="24"/>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="18"/>
-      <c r="Y31" s="18"/>
-      <c r="Z31" s="18"/>
-      <c r="AA31" s="18"/>
-      <c r="AC31" s="30" t="s">
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="Y30" s="24"/>
+      <c r="Z30" s="24"/>
+      <c r="AA30" s="24"/>
+      <c r="AL30" s="12"/>
+    </row>
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
+      <c r="Z31" s="24"/>
+      <c r="AA31" s="24"/>
+      <c r="AC31" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="AD31" s="22" t="s">
+      <c r="AD31" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="AE31" s="22"/>
-      <c r="AF31" s="22"/>
-      <c r="AG31" s="22"/>
-      <c r="AH31" s="22"/>
-      <c r="AI31" s="22"/>
-      <c r="AJ31" s="22"/>
-      <c r="AL31" s="24"/>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AE31" s="21"/>
+      <c r="AF31" s="21"/>
+      <c r="AG31" s="21"/>
+      <c r="AH31" s="21"/>
+      <c r="AI31" s="21"/>
+      <c r="AJ31" s="21"/>
+      <c r="AL31" s="12"/>
+    </row>
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="H32" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="J32" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="18"/>
-      <c r="AC32" s="30"/>
-      <c r="AD32" s="22"/>
-      <c r="AE32" s="22"/>
-      <c r="AF32" s="22"/>
-      <c r="AG32" s="22"/>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="22"/>
-      <c r="AJ32" s="22"/>
-      <c r="AL32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="24"/>
+      <c r="Z32" s="24"/>
+      <c r="AA32" s="24"/>
+      <c r="AC32" s="22"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="21"/>
+      <c r="AF32" s="21"/>
+      <c r="AG32" s="21"/>
+      <c r="AH32" s="21"/>
+      <c r="AI32" s="21"/>
+      <c r="AJ32" s="21"/>
+      <c r="AL32" s="12"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="18"/>
-      <c r="Y33" s="18"/>
-      <c r="Z33" s="18"/>
-      <c r="AA33" s="18"/>
-      <c r="AC33" s="30"/>
-      <c r="AD33" s="22"/>
-      <c r="AE33" s="22"/>
-      <c r="AF33" s="22"/>
-      <c r="AG33" s="22"/>
-      <c r="AH33" s="22"/>
-      <c r="AI33" s="22"/>
-      <c r="AJ33" s="22"/>
-      <c r="AL33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="21"/>
+      <c r="AE33" s="21"/>
+      <c r="AF33" s="21"/>
+      <c r="AG33" s="21"/>
+      <c r="AH33" s="21"/>
+      <c r="AI33" s="21"/>
+      <c r="AJ33" s="21"/>
+      <c r="AL33" s="12"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="W34" s="18"/>
-      <c r="X34" s="18"/>
-      <c r="Y34" s="18"/>
-      <c r="Z34" s="18"/>
-      <c r="AA34" s="18"/>
-      <c r="AL34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="W34" s="24"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="24"/>
+      <c r="Z34" s="24"/>
+      <c r="AA34" s="24"/>
+      <c r="AL34" s="12"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="H35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="W35" s="18"/>
-      <c r="X35" s="18"/>
-      <c r="Y35" s="18"/>
-      <c r="Z35" s="18"/>
-      <c r="AA35" s="18"/>
-      <c r="AL35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="W35" s="24"/>
+      <c r="X35" s="24"/>
+      <c r="Y35" s="24"/>
+      <c r="Z35" s="24"/>
+      <c r="AA35" s="24"/>
+      <c r="AL35" s="12"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="18"/>
-      <c r="Y36" s="18"/>
-      <c r="Z36" s="18"/>
-      <c r="AA36" s="18"/>
-      <c r="AL36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24"/>
+      <c r="Z36" s="24"/>
+      <c r="AA36" s="24"/>
+      <c r="AL36" s="12"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="W37" s="18"/>
-      <c r="X37" s="18"/>
-      <c r="Y37" s="18"/>
-      <c r="Z37" s="18"/>
-      <c r="AA37" s="18"/>
-      <c r="AL37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="W37" s="24"/>
+      <c r="X37" s="24"/>
+      <c r="Y37" s="24"/>
+      <c r="Z37" s="24"/>
+      <c r="AA37" s="24"/>
+      <c r="AL37" s="12"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="18"/>
-      <c r="Y38" s="18"/>
-      <c r="Z38" s="18"/>
-      <c r="AA38" s="18"/>
-      <c r="AL38" s="24"/>
+      <c r="A38" s="10"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+      <c r="Y38" s="24"/>
+      <c r="Z38" s="24"/>
+      <c r="AA38" s="24"/>
+      <c r="AL38" s="12"/>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-      <c r="Y39" s="18"/>
-      <c r="Z39" s="18"/>
-      <c r="AA39" s="18"/>
-      <c r="AL39" s="24"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="W39" s="24"/>
+      <c r="X39" s="24"/>
+      <c r="Y39" s="24"/>
+      <c r="Z39" s="24"/>
+      <c r="AA39" s="24"/>
+      <c r="AL39" s="12"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="W40" s="18"/>
-      <c r="X40" s="18"/>
-      <c r="Y40" s="18"/>
-      <c r="Z40" s="18"/>
-      <c r="AA40" s="18"/>
-      <c r="AL40" s="24"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="24"/>
+      <c r="Z40" s="24"/>
+      <c r="AA40" s="24"/>
+      <c r="AL40" s="12"/>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="W41" s="18"/>
-      <c r="X41" s="18"/>
-      <c r="Y41" s="18"/>
-      <c r="Z41" s="18"/>
-      <c r="AA41" s="18"/>
-      <c r="AL41" s="24"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="24"/>
+      <c r="Z41" s="24"/>
+      <c r="AA41" s="24"/>
+      <c r="AL41" s="12"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
@@ -3602,124 +3740,124 @@
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
       <c r="M42" s="19"/>
-      <c r="N42" s="20"/>
-      <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
-      <c r="Y42" s="26"/>
-      <c r="Z42" s="26"/>
-      <c r="AA42" s="26"/>
-      <c r="AL42" s="24"/>
+      <c r="N42" s="9"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AL42" s="12"/>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="20"/>
-      <c r="W43" s="26"/>
-      <c r="X43" s="26"/>
-      <c r="Y43" s="26"/>
-      <c r="Z43" s="26"/>
-      <c r="AA43" s="26"/>
-      <c r="AL43" s="24"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="9"/>
+      <c r="W43" s="14"/>
+      <c r="X43" s="14"/>
+      <c r="Y43" s="14"/>
+      <c r="Z43" s="14"/>
+      <c r="AA43" s="14"/>
+      <c r="AL43" s="12"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="20"/>
-      <c r="AL44" s="24"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="9"/>
+      <c r="AL44" s="12"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="AL45" s="24"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="AL45" s="12"/>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="24"/>
-      <c r="P46" s="24"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
-      <c r="T46" s="24"/>
-      <c r="U46" s="24"/>
-      <c r="V46" s="24"/>
-      <c r="W46" s="24"/>
-      <c r="X46" s="24"/>
-      <c r="Y46" s="24"/>
-      <c r="Z46" s="24"/>
-      <c r="AA46" s="24"/>
-      <c r="AB46" s="24"/>
-      <c r="AC46" s="24"/>
-      <c r="AD46" s="24"/>
-      <c r="AE46" s="24"/>
-      <c r="AF46" s="24"/>
-      <c r="AG46" s="24"/>
-      <c r="AH46" s="24"/>
-      <c r="AI46" s="24"/>
-      <c r="AJ46" s="24"/>
-      <c r="AK46" s="24"/>
-      <c r="AL46" s="24"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AD46" s="12"/>
+      <c r="AE46" s="12"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AH46" s="12"/>
+      <c r="AI46" s="12"/>
+      <c r="AJ46" s="12"/>
+      <c r="AK46" s="12"/>
+      <c r="AL46" s="12"/>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="AL47" s="24"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="AL47" s="12"/>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
       <c r="H48" t="s">
         <v>70</v>
       </c>
@@ -3744,15 +3882,15 @@
       <c r="O48" t="s">
         <v>55</v>
       </c>
-      <c r="AL48" s="24"/>
+      <c r="AL48" s="12"/>
     </row>
     <row r="49" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
       <c r="H49">
         <v>1</v>
       </c>
@@ -3763,20 +3901,20 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="Q49" s="20"/>
-      <c r="R49" s="20"/>
-      <c r="S49" s="20"/>
-      <c r="T49" s="20"/>
-      <c r="U49" s="20"/>
-      <c r="AL49" s="24"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+      <c r="AL49" s="12"/>
     </row>
     <row r="50" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
       <c r="H50">
         <v>2</v>
       </c>
@@ -3787,22 +3925,22 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="Q50" s="16" t="s">
+      <c r="Q50" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="R50" s="16"/>
-      <c r="S50" s="16"/>
-      <c r="T50" s="16"/>
-      <c r="U50" s="16"/>
-      <c r="AL50" s="24"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="26"/>
+      <c r="T50" s="26"/>
+      <c r="U50" s="26"/>
+      <c r="AL50" s="12"/>
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
       <c r="H51">
         <v>3</v>
       </c>
@@ -3813,22 +3951,22 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-      <c r="Q51" s="16" t="s">
+      <c r="Q51" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="R51" s="16"/>
-      <c r="S51" s="16"/>
-      <c r="T51" s="16"/>
-      <c r="U51" s="16"/>
-      <c r="AL51" s="24"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="AL51" s="12"/>
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
       <c r="H52" t="s">
         <v>41</v>
       </c>
@@ -3839,20 +3977,20 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
-      <c r="Q52" s="16"/>
-      <c r="R52" s="16"/>
-      <c r="S52" s="16"/>
-      <c r="T52" s="16"/>
-      <c r="U52" s="16"/>
-      <c r="AL52" s="24"/>
+      <c r="Q52" s="26"/>
+      <c r="R52" s="26"/>
+      <c r="S52" s="26"/>
+      <c r="T52" s="26"/>
+      <c r="U52" s="26"/>
+      <c r="AL52" s="12"/>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
       <c r="H53">
         <v>24</v>
       </c>
@@ -3863,94 +4001,94 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
-      <c r="Q53" s="16"/>
-      <c r="R53" s="16"/>
-      <c r="S53" s="16"/>
-      <c r="T53" s="16"/>
-      <c r="U53" s="16"/>
-      <c r="AL53" s="24"/>
+      <c r="Q53" s="26"/>
+      <c r="R53" s="26"/>
+      <c r="S53" s="26"/>
+      <c r="T53" s="26"/>
+      <c r="U53" s="26"/>
+      <c r="AL53" s="12"/>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="Q54" s="16"/>
-      <c r="R54" s="16"/>
-      <c r="S54" s="16"/>
-      <c r="T54" s="16"/>
-      <c r="U54" s="16"/>
-      <c r="AL54" s="24"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="Q54" s="26"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="26"/>
+      <c r="T54" s="26"/>
+      <c r="U54" s="26"/>
+      <c r="AL54" s="12"/>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
-      <c r="S55" s="16"/>
-      <c r="T55" s="16"/>
-      <c r="U55" s="16"/>
-      <c r="AL55" s="24"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="Q55" s="26"/>
+      <c r="R55" s="26"/>
+      <c r="S55" s="26"/>
+      <c r="T55" s="26"/>
+      <c r="U55" s="26"/>
+      <c r="AL55" s="12"/>
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="Q56" s="16"/>
-      <c r="R56" s="16"/>
-      <c r="S56" s="16"/>
-      <c r="T56" s="16"/>
-      <c r="U56" s="16"/>
-      <c r="AL56" s="24"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="Q56" s="26"/>
+      <c r="R56" s="26"/>
+      <c r="S56" s="26"/>
+      <c r="T56" s="26"/>
+      <c r="U56" s="26"/>
+      <c r="AL56" s="12"/>
     </row>
     <row r="57" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="16"/>
-      <c r="S57" s="16"/>
-      <c r="T57" s="16"/>
-      <c r="U57" s="16"/>
-      <c r="AL57" s="24"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="Q57" s="26"/>
+      <c r="R57" s="26"/>
+      <c r="S57" s="26"/>
+      <c r="T57" s="26"/>
+      <c r="U57" s="26"/>
+      <c r="AL57" s="12"/>
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Q58" s="16"/>
-      <c r="R58" s="16"/>
-      <c r="S58" s="16"/>
-      <c r="T58" s="16"/>
-      <c r="U58" s="16"/>
-      <c r="AL58" s="24"/>
+      <c r="Q58" s="26"/>
+      <c r="R58" s="26"/>
+      <c r="S58" s="26"/>
+      <c r="T58" s="26"/>
+      <c r="U58" s="26"/>
+      <c r="AL58" s="12"/>
     </row>
     <row r="59" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Q59" s="16"/>
-      <c r="R59" s="16"/>
-      <c r="S59" s="16"/>
-      <c r="T59" s="16"/>
-      <c r="U59" s="16"/>
-      <c r="AL59" s="24"/>
+      <c r="Q59" s="26"/>
+      <c r="R59" s="26"/>
+      <c r="S59" s="26"/>
+      <c r="T59" s="26"/>
+      <c r="U59" s="26"/>
+      <c r="AL59" s="12"/>
     </row>
     <row r="60" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Q60" s="20"/>
-      <c r="AL60" s="24"/>
+      <c r="Q60" s="9"/>
+      <c r="AL60" s="12"/>
     </row>
     <row r="61" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL61" s="24"/>
+      <c r="AL61" s="12"/>
     </row>
     <row r="62" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL62" s="24"/>
+      <c r="AL62" s="12"/>
     </row>
     <row r="63" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
@@ -3968,98 +4106,122 @@
       <c r="K63" s="19"/>
       <c r="L63" s="19"/>
       <c r="M63" s="19"/>
-      <c r="AL63" s="24"/>
+      <c r="AL63" s="12"/>
     </row>
     <row r="64" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="27" t="s">
+      <c r="B64" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="27"/>
-      <c r="M64" s="27"/>
-      <c r="AL64" s="24"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="AL64" s="12"/>
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
-      <c r="J65" s="27"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
-      <c r="AL65" s="24"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="AL65" s="12"/>
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL66" s="24"/>
+      <c r="AL66" s="12"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL67" s="24"/>
+      <c r="AL67" s="12"/>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL68" s="24"/>
+      <c r="AL68" s="12"/>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL69" s="24"/>
+      <c r="AL69" s="12"/>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
-      <c r="J70" s="24"/>
-      <c r="K70" s="24"/>
-      <c r="L70" s="24"/>
-      <c r="M70" s="24"/>
-      <c r="N70" s="24"/>
-      <c r="O70" s="24"/>
-      <c r="P70" s="24"/>
-      <c r="Q70" s="24"/>
-      <c r="R70" s="24"/>
-      <c r="S70" s="24"/>
-      <c r="T70" s="24"/>
-      <c r="U70" s="24"/>
-      <c r="V70" s="24"/>
-      <c r="W70" s="24"/>
-      <c r="X70" s="24"/>
-      <c r="Y70" s="24"/>
-      <c r="Z70" s="24"/>
-      <c r="AA70" s="24"/>
-      <c r="AB70" s="24"/>
-      <c r="AC70" s="24"/>
-      <c r="AD70" s="24"/>
-      <c r="AE70" s="24"/>
-      <c r="AF70" s="24"/>
-      <c r="AG70" s="24"/>
-      <c r="AH70" s="24"/>
-      <c r="AI70" s="24"/>
-      <c r="AJ70" s="24"/>
-      <c r="AK70" s="24"/>
-      <c r="AL70" s="24"/>
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+      <c r="P70" s="12"/>
+      <c r="Q70" s="12"/>
+      <c r="R70" s="12"/>
+      <c r="S70" s="12"/>
+      <c r="T70" s="12"/>
+      <c r="U70" s="12"/>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="X70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="Z70" s="12"/>
+      <c r="AA70" s="12"/>
+      <c r="AB70" s="12"/>
+      <c r="AC70" s="12"/>
+      <c r="AD70" s="12"/>
+      <c r="AE70" s="12"/>
+      <c r="AF70" s="12"/>
+      <c r="AG70" s="12"/>
+      <c r="AH70" s="12"/>
+      <c r="AI70" s="12"/>
+      <c r="AJ70" s="12"/>
+      <c r="AK70" s="12"/>
+      <c r="AL70" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="36">
+    <mergeCell ref="AO3:BD3"/>
+    <mergeCell ref="AO23:BD23"/>
+    <mergeCell ref="B3:F12"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B21:F30"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="O5:S15"/>
+    <mergeCell ref="O4:S4"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O22:S39"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:M17"/>
+    <mergeCell ref="AD25:AJ25"/>
+    <mergeCell ref="AD27:AJ28"/>
+    <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="W21:AA21"/>
+    <mergeCell ref="W22:AA41"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="I35:M35"/>
+    <mergeCell ref="J30:M31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="H30:H31"/>
     <mergeCell ref="A63:M63"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B64:M65"/>
@@ -4068,32 +4230,10 @@
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:M44"/>
     <mergeCell ref="A42:M42"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:M17"/>
-    <mergeCell ref="AD25:AJ25"/>
-    <mergeCell ref="AD27:AJ28"/>
-    <mergeCell ref="AC27:AC28"/>
     <mergeCell ref="B48:F57"/>
-    <mergeCell ref="W21:AA21"/>
-    <mergeCell ref="W22:AA41"/>
     <mergeCell ref="A48:A57"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="I35:M35"/>
     <mergeCell ref="Q51:U59"/>
     <mergeCell ref="Q50:U50"/>
-    <mergeCell ref="J30:M31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="O5:S15"/>
-    <mergeCell ref="O4:S4"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O22:S39"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="B3:F12"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="B21:F30"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="A15:M15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HOJA2(excel) ESTRUCUTRA PARA LA INFO DE ACTIVIDADES COTIDIANAS DEL USUARIO Y FORMATO DE SALVADO
</commit_message>
<xml_diff>
--- a/ANALISIS  DEL PROBLEMA/horario y materiras.xlsx
+++ b/ANALISIS  DEL PROBLEMA/horario y materiras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\INFO II\TEORIA\PARCIAL 1 - ANDRES RIVERA\ANALISIS  DEL PROBLEMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012C21D9-E5A3-4BC2-8A43-662162E6AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB6F5F1-B91D-4543-83C4-E7867FDB027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -362,9 +362,6 @@
     <t>(13/14-04-2023) Se agrega formato de texto parala informacion de cada curso correspondiente. A las cursos de un credito se les asignará un total de 5 horas semanales, las cuales se repartiran entre las HTD y HTP</t>
   </si>
   <si>
-    <t>CUADRAR HORAS DE SUEÑO Y ALIMENTACIÓN y dudas si agrega la contraseña al usuario</t>
-  </si>
-  <si>
     <t>MANEJO DE LA INFORMACIÓN CURSOS</t>
   </si>
   <si>
@@ -372,6 +369,46 @@
   </si>
   <si>
     <t>NOTA: si algo se tiene pensado en separar el nombre del curso en otro arreglo, de momento se va a amnejar de esta forma como se planteo.</t>
+  </si>
+  <si>
+    <t>CAMBIO2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(14-04-2023)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Se grega al archivo horaio estudiantes, la parte de el horario que seran filas(7 por ser 7 dias de la semana) y las 3 primeras parejas de ceros separadas por coma, seran horario de las tres comida; y las ultimas seran las de horas para dormir. Además se agrega otro arreglo que sera de apoyo para guardar esta información.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dudas si agrega la contraseña al usuario</t>
   </si>
 </sst>
 </file>
@@ -453,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -513,11 +550,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -551,29 +625,20 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -584,11 +649,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,50 +745,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>268627</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>122574</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>511969</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>115104</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ED65D81-80F3-454F-A193-D8591DB68F8D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11746252" y="3170574"/>
-          <a:ext cx="3291342" cy="3231030"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>119062</xdr:colOff>
       <xdr:row>21</xdr:row>
@@ -724,7 +770,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -768,7 +814,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -812,7 +858,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:srcRect b="22020"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -824,6 +870,98 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>640109</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>144683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>154781</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6CD1D8-3064-41F9-AD68-E0D5563734C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect b="8944"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12117734" y="4204714"/>
+          <a:ext cx="2562672" cy="4046317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>750094</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>729522</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>2138</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C24647-A8F1-4FDE-BC2E-2602C86293D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30801469" y="7072312"/>
+          <a:ext cx="12171428" cy="1942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2809,6 +2947,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
     <mergeCell ref="A96:A99"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="A104:A107"/>
@@ -2825,26 +2983,6 @@
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A60:A63"/>
     <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2853,10 +2991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C3E2EB-B927-45CA-9B97-F8A6A5130907}">
-  <dimension ref="A1:BD70"/>
+  <dimension ref="A1:BD74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AK1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AS19" sqref="AS19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AM20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AM42" sqref="AM42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2911,59 +3049,59 @@
       <c r="AL2" s="12"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="AL3" s="12"/>
-      <c r="AO3" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP3" s="31"/>
-      <c r="AQ3" s="31"/>
-      <c r="AR3" s="31"/>
-      <c r="AS3" s="31"/>
-      <c r="AT3" s="31"/>
-      <c r="AU3" s="31"/>
-      <c r="AV3" s="31"/>
-      <c r="AW3" s="31"/>
-      <c r="AX3" s="31"/>
-      <c r="AY3" s="31"/>
-      <c r="AZ3" s="31"/>
-      <c r="BA3" s="31"/>
-      <c r="BB3" s="31"/>
-      <c r="BC3" s="31"/>
-      <c r="BD3" s="31"/>
+      <c r="AO3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AW3" s="19"/>
+      <c r="AX3" s="19"/>
+      <c r="AY3" s="19"/>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="19"/>
+      <c r="BB3" s="19"/>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="O4" s="19" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="O4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
       <c r="AL4" s="12"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
       <c r="H5" t="s">
         <v>40</v>
       </c>
@@ -2982,20 +3120,20 @@
       <c r="M5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
       <c r="AL5" s="12"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
       <c r="H6" t="s">
         <v>41</v>
       </c>
@@ -3004,20 +3142,20 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
       <c r="AL6" s="12"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
       <c r="H7" t="s">
         <v>42</v>
       </c>
@@ -3026,159 +3164,159 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
       <c r="AL7" s="12"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
       <c r="AL8" s="12"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
       <c r="AL9" s="12"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
       <c r="AL10" s="12"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
       <c r="AL11" s="12"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
       <c r="AL12" s="12"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
       <c r="AL13" s="12"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
       <c r="AL14" s="12"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
       <c r="AL15" s="12"/>
     </row>
     <row r="16" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
       <c r="AL16" s="12"/>
       <c r="AO16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
       <c r="AL17" s="12"/>
     </row>
     <row r="18" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3228,106 +3366,106 @@
       <c r="AL20" s="12"/>
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="O21" s="19" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="O21" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="W21" s="19" t="s">
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="W21" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="22"/>
       <c r="AL21" s="12"/>
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
       <c r="AL22" s="12"/>
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
       <c r="H23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="28"/>
-      <c r="L23" s="29"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
       <c r="AL23" s="12"/>
-      <c r="AO23" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP23" s="31"/>
-      <c r="AQ23" s="31"/>
-      <c r="AR23" s="31"/>
-      <c r="AS23" s="31"/>
-      <c r="AT23" s="31"/>
-      <c r="AU23" s="31"/>
-      <c r="AV23" s="31"/>
-      <c r="AW23" s="31"/>
-      <c r="AX23" s="31"/>
-      <c r="AY23" s="31"/>
-      <c r="AZ23" s="31"/>
-      <c r="BA23" s="31"/>
-      <c r="BB23" s="31"/>
-      <c r="BC23" s="31"/>
-      <c r="BD23" s="31"/>
+      <c r="AO23" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP23" s="22"/>
+      <c r="AQ23" s="22"/>
+      <c r="AR23" s="22"/>
+      <c r="AS23" s="22"/>
+      <c r="AT23" s="22"/>
+      <c r="AU23" s="22"/>
+      <c r="AV23" s="22"/>
+      <c r="AW23" s="22"/>
+      <c r="AX23" s="22"/>
+      <c r="AY23" s="22"/>
+      <c r="AZ23" s="22"/>
+      <c r="BA23" s="22"/>
+      <c r="BB23" s="22"/>
+      <c r="BC23" s="22"/>
+      <c r="BD23" s="22"/>
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="H24" s="1" t="s">
         <v>50</v>
       </c>
@@ -3343,211 +3481,211 @@
       <c r="L24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="24"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
       <c r="AL24" s="12"/>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-      <c r="AA25" s="24"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
       <c r="AC25" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AD25" s="24" t="s">
+      <c r="AD25" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="AE25" s="24"/>
-      <c r="AF25" s="24"/>
-      <c r="AG25" s="24"/>
-      <c r="AH25" s="24"/>
-      <c r="AI25" s="24"/>
-      <c r="AJ25" s="24"/>
+      <c r="AE25" s="23"/>
+      <c r="AF25" s="23"/>
+      <c r="AG25" s="23"/>
+      <c r="AH25" s="23"/>
+      <c r="AI25" s="23"/>
+      <c r="AJ25" s="23"/>
       <c r="AL25" s="12"/>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="24"/>
-      <c r="AA26" s="24"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="23"/>
       <c r="AL26" s="12"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AC27" s="25" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AC27" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="AD27" s="21" t="s">
+      <c r="AD27" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AE27" s="21"/>
-      <c r="AF27" s="21"/>
-      <c r="AG27" s="21"/>
-      <c r="AH27" s="21"/>
-      <c r="AI27" s="21"/>
-      <c r="AJ27" s="21"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="28"/>
+      <c r="AG27" s="28"/>
+      <c r="AH27" s="28"/>
+      <c r="AI27" s="28"/>
+      <c r="AJ27" s="28"/>
       <c r="AL27" s="12"/>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="24"/>
-      <c r="AC28" s="25"/>
-      <c r="AD28" s="21"/>
-      <c r="AE28" s="21"/>
-      <c r="AF28" s="21"/>
-      <c r="AG28" s="21"/>
-      <c r="AH28" s="21"/>
-      <c r="AI28" s="21"/>
-      <c r="AJ28" s="21"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AC28" s="29"/>
+      <c r="AD28" s="28"/>
+      <c r="AE28" s="28"/>
+      <c r="AF28" s="28"/>
+      <c r="AG28" s="28"/>
+      <c r="AH28" s="28"/>
+      <c r="AI28" s="28"/>
+      <c r="AJ28" s="28"/>
       <c r="AL28" s="12"/>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
       <c r="H29" t="s">
         <v>72</v>
       </c>
       <c r="I29" t="s">
         <v>73</v>
       </c>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="24"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
       <c r="AL29" s="12"/>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="H30" s="21" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="H30" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="J30" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="24"/>
-      <c r="AA30" s="24"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
+      <c r="AA30" s="23"/>
       <c r="AL30" s="12"/>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AC31" s="22" t="s">
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23"/>
+      <c r="W31" s="23"/>
+      <c r="X31" s="23"/>
+      <c r="Y31" s="23"/>
+      <c r="Z31" s="23"/>
+      <c r="AA31" s="23"/>
+      <c r="AC31" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="AD31" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE31" s="21"/>
-      <c r="AF31" s="21"/>
-      <c r="AG31" s="21"/>
-      <c r="AH31" s="21"/>
-      <c r="AI31" s="21"/>
-      <c r="AJ31" s="21"/>
+      <c r="AD31" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE31" s="28"/>
+      <c r="AF31" s="28"/>
+      <c r="AG31" s="28"/>
+      <c r="AH31" s="28"/>
+      <c r="AI31" s="28"/>
+      <c r="AJ31" s="28"/>
       <c r="AL31" s="12"/>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
@@ -3557,442 +3695,515 @@
       <c r="I32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="24" t="s">
+      <c r="J32" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
-      <c r="Z32" s="24"/>
-      <c r="AA32" s="24"/>
-      <c r="AC32" s="22"/>
-      <c r="AD32" s="21"/>
-      <c r="AE32" s="21"/>
-      <c r="AF32" s="21"/>
-      <c r="AG32" s="21"/>
-      <c r="AH32" s="21"/>
-      <c r="AI32" s="21"/>
-      <c r="AJ32" s="21"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AC32" s="31"/>
+      <c r="AD32" s="28"/>
+      <c r="AE32" s="28"/>
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="28"/>
+      <c r="AH32" s="28"/>
+      <c r="AI32" s="28"/>
+      <c r="AJ32" s="28"/>
       <c r="AL32" s="12"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="24"/>
-      <c r="AA33" s="24"/>
-      <c r="AC33" s="22"/>
-      <c r="AD33" s="21"/>
-      <c r="AE33" s="21"/>
-      <c r="AF33" s="21"/>
-      <c r="AG33" s="21"/>
-      <c r="AH33" s="21"/>
-      <c r="AI33" s="21"/>
-      <c r="AJ33" s="21"/>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
+      <c r="AA33" s="23"/>
+      <c r="AC33" s="31"/>
+      <c r="AD33" s="28"/>
+      <c r="AE33" s="28"/>
+      <c r="AF33" s="28"/>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="28"/>
+      <c r="AI33" s="28"/>
+      <c r="AJ33" s="28"/>
       <c r="AL33" s="12"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="24"/>
-      <c r="Z34" s="24"/>
-      <c r="AA34" s="24"/>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="23"/>
+      <c r="AA34" s="23"/>
       <c r="AL34" s="12"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="H35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="24" t="s">
+      <c r="I35" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="W35" s="24"/>
-      <c r="X35" s="24"/>
-      <c r="Y35" s="24"/>
-      <c r="Z35" s="24"/>
-      <c r="AA35" s="24"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+      <c r="Y35" s="23"/>
+      <c r="Z35" s="23"/>
+      <c r="AA35" s="23"/>
       <c r="AL35" s="12"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="W36" s="24"/>
-      <c r="X36" s="24"/>
-      <c r="Y36" s="24"/>
-      <c r="Z36" s="24"/>
-      <c r="AA36" s="24"/>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="23"/>
       <c r="AL36" s="12"/>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="W37" s="24"/>
-      <c r="X37" s="24"/>
-      <c r="Y37" s="24"/>
-      <c r="Z37" s="24"/>
-      <c r="AA37" s="24"/>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="23"/>
+      <c r="Y37" s="23"/>
+      <c r="Z37" s="23"/>
+      <c r="AA37" s="23"/>
       <c r="AL37" s="12"/>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN37" s="34"/>
+      <c r="AO37" s="34"/>
+      <c r="AP37" s="34"/>
+      <c r="AQ37" s="34"/>
+      <c r="AR37" s="34"/>
+      <c r="AS37" s="34"/>
+      <c r="AT37" s="34"/>
+      <c r="AU37" s="34"/>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="24"/>
-      <c r="W38" s="24"/>
-      <c r="X38" s="24"/>
-      <c r="Y38" s="24"/>
-      <c r="Z38" s="24"/>
-      <c r="AA38" s="24"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="W38" s="23"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="23"/>
+      <c r="AA38" s="23"/>
       <c r="AL38" s="12"/>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN38" s="34"/>
+      <c r="AO38" s="34"/>
+      <c r="AP38" s="34"/>
+      <c r="AQ38" s="34"/>
+      <c r="AR38" s="34"/>
+      <c r="AS38" s="34"/>
+      <c r="AT38" s="34"/>
+      <c r="AU38" s="34"/>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="O39" s="24"/>
-      <c r="P39" s="24"/>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="24"/>
-      <c r="S39" s="24"/>
-      <c r="W39" s="24"/>
-      <c r="X39" s="24"/>
-      <c r="Y39" s="24"/>
-      <c r="Z39" s="24"/>
-      <c r="AA39" s="24"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="W39" s="23"/>
+      <c r="X39" s="23"/>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="23"/>
+      <c r="AA39" s="23"/>
       <c r="AL39" s="12"/>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN39" s="34"/>
+      <c r="AO39" s="34"/>
+      <c r="AP39" s="34"/>
+      <c r="AQ39" s="34"/>
+      <c r="AR39" s="34"/>
+      <c r="AS39" s="34"/>
+      <c r="AT39" s="34"/>
+      <c r="AU39" s="34"/>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="W40" s="24"/>
-      <c r="X40" s="24"/>
-      <c r="Y40" s="24"/>
-      <c r="Z40" s="24"/>
-      <c r="AA40" s="24"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
+      <c r="AA40" s="23"/>
       <c r="AL40" s="12"/>
-    </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN40" s="34"/>
+      <c r="AO40" s="34"/>
+      <c r="AP40" s="34"/>
+      <c r="AQ40" s="34"/>
+      <c r="AR40" s="34"/>
+      <c r="AS40" s="34"/>
+      <c r="AT40" s="34"/>
+      <c r="AU40" s="34"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="W41" s="24"/>
-      <c r="X41" s="24"/>
-      <c r="Y41" s="24"/>
-      <c r="Z41" s="24"/>
-      <c r="AA41" s="24"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
+      <c r="Z41" s="23"/>
+      <c r="AA41" s="23"/>
       <c r="AL41" s="12"/>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="AN41" s="34"/>
+      <c r="AO41" s="34"/>
+      <c r="AP41" s="34"/>
+      <c r="AQ41" s="34"/>
+      <c r="AR41" s="34"/>
+      <c r="AS41" s="34"/>
+      <c r="AT41" s="34"/>
+      <c r="AU41" s="34"/>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
       <c r="N42" s="9"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="23"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="23"/>
       <c r="W42" s="14"/>
       <c r="X42" s="14"/>
       <c r="Y42" s="14"/>
       <c r="Z42" s="14"/>
       <c r="AA42" s="14"/>
       <c r="AL42" s="12"/>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="AN42" s="34"/>
+      <c r="AO42" s="34"/>
+      <c r="AP42" s="34"/>
+      <c r="AQ42" s="34"/>
+      <c r="AR42" s="34"/>
+      <c r="AS42" s="34"/>
+      <c r="AT42" s="34"/>
+      <c r="AU42" s="34"/>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="30"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="30"/>
       <c r="N43" s="9"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
       <c r="W43" s="14"/>
       <c r="X43" s="14"/>
       <c r="Y43" s="14"/>
       <c r="Z43" s="14"/>
       <c r="AA43" s="14"/>
       <c r="AL43" s="12"/>
-    </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
+      <c r="AN43" s="34"/>
+      <c r="AO43" s="34"/>
+      <c r="AP43" s="34"/>
+      <c r="AQ43" s="34"/>
+      <c r="AR43" s="34"/>
+      <c r="AS43" s="34"/>
+      <c r="AT43" s="34"/>
+      <c r="AU43" s="34"/>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="30"/>
+      <c r="M44" s="30"/>
       <c r="N44" s="9"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
       <c r="AL44" s="12"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
+    <row r="45" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
       <c r="AL45" s="12"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="12"/>
-      <c r="Q46" s="12"/>
-      <c r="R46" s="12"/>
-      <c r="S46" s="12"/>
-      <c r="T46" s="12"/>
-      <c r="U46" s="12"/>
-      <c r="V46" s="12"/>
-      <c r="W46" s="12"/>
-      <c r="X46" s="12"/>
-      <c r="Y46" s="12"/>
-      <c r="Z46" s="12"/>
-      <c r="AA46" s="12"/>
-      <c r="AB46" s="12"/>
-      <c r="AC46" s="12"/>
-      <c r="AD46" s="12"/>
-      <c r="AE46" s="12"/>
-      <c r="AF46" s="12"/>
-      <c r="AG46" s="12"/>
-      <c r="AH46" s="12"/>
-      <c r="AI46" s="12"/>
-      <c r="AJ46" s="12"/>
-      <c r="AK46" s="12"/>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A46" s="36"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
       <c r="AL46" s="12"/>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A47" s="37"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
       <c r="AL47" s="12"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="AL48" s="12"/>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="AL49" s="12"/>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="12"/>
+      <c r="V50" s="12"/>
+      <c r="W50" s="12"/>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="12"/>
+      <c r="Z50" s="12"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="12"/>
+      <c r="AC50" s="12"/>
+      <c r="AD50" s="12"/>
+      <c r="AE50" s="12"/>
+      <c r="AF50" s="12"/>
+      <c r="AG50" s="12"/>
+      <c r="AH50" s="12"/>
+      <c r="AI50" s="12"/>
+      <c r="AJ50" s="12"/>
+      <c r="AK50" s="12"/>
+      <c r="AL50" s="12"/>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="AL51" s="12"/>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B52" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="H48" t="s">
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="H52" t="s">
         <v>70</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I52" t="s">
         <v>46</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J52" t="s">
         <v>47</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K52" t="s">
         <v>48</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L52" t="s">
         <v>52</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M52" t="s">
         <v>53</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N52" t="s">
         <v>54</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O52" t="s">
         <v>55</v>
       </c>
-      <c r="AL48" s="12"/>
-    </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="H49">
+      <c r="AL52" s="12"/>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="H53">
         <v>1</v>
-      </c>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
-      <c r="AL49" s="12"/>
-    </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="H50">
-        <v>2</v>
-      </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="Q50" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="R50" s="26"/>
-      <c r="S50" s="26"/>
-      <c r="T50" s="26"/>
-      <c r="U50" s="26"/>
-      <c r="AL50" s="12"/>
-    </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="H51">
-        <v>3</v>
-      </c>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="Q51" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="R51" s="26"/>
-      <c r="S51" s="26"/>
-      <c r="T51" s="26"/>
-      <c r="U51" s="26"/>
-      <c r="AL51" s="12"/>
-    </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="H52" t="s">
-        <v>41</v>
-      </c>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="Q52" s="26"/>
-      <c r="R52" s="26"/>
-      <c r="S52" s="26"/>
-      <c r="T52" s="26"/>
-      <c r="U52" s="26"/>
-      <c r="AL52" s="12"/>
-    </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="H53">
-        <v>24</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -4001,203 +4212,326 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
-      <c r="Q53" s="26"/>
-      <c r="R53" s="26"/>
-      <c r="S53" s="26"/>
-      <c r="T53" s="26"/>
-      <c r="U53" s="26"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="9"/>
       <c r="AL53" s="12"/>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="Q54" s="26"/>
-      <c r="R54" s="26"/>
-      <c r="S54" s="26"/>
-      <c r="T54" s="26"/>
-      <c r="U54" s="26"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="Q54" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="R54" s="20"/>
+      <c r="S54" s="20"/>
+      <c r="T54" s="20"/>
+      <c r="U54" s="20"/>
       <c r="AL54" s="12"/>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="Q55" s="26"/>
-      <c r="R55" s="26"/>
-      <c r="S55" s="26"/>
-      <c r="T55" s="26"/>
-      <c r="U55" s="26"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="Q55" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="R55" s="20"/>
+      <c r="S55" s="20"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="20"/>
       <c r="AL55" s="12"/>
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="Q56" s="26"/>
-      <c r="R56" s="26"/>
-      <c r="S56" s="26"/>
-      <c r="T56" s="26"/>
-      <c r="U56" s="26"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="H56" t="s">
+        <v>41</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="20"/>
+      <c r="S56" s="20"/>
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
       <c r="AL56" s="12"/>
     </row>
     <row r="57" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="Q57" s="26"/>
-      <c r="R57" s="26"/>
-      <c r="S57" s="26"/>
-      <c r="T57" s="26"/>
-      <c r="U57" s="26"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="H57">
+        <v>24</v>
+      </c>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="20"/>
+      <c r="T57" s="20"/>
+      <c r="U57" s="20"/>
       <c r="AL57" s="12"/>
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Q58" s="26"/>
-      <c r="R58" s="26"/>
-      <c r="S58" s="26"/>
-      <c r="T58" s="26"/>
-      <c r="U58" s="26"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="20"/>
+      <c r="T58" s="20"/>
+      <c r="U58" s="20"/>
       <c r="AL58" s="12"/>
     </row>
     <row r="59" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Q59" s="26"/>
-      <c r="R59" s="26"/>
-      <c r="S59" s="26"/>
-      <c r="T59" s="26"/>
-      <c r="U59" s="26"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="Q59" s="20"/>
+      <c r="R59" s="20"/>
+      <c r="S59" s="20"/>
+      <c r="T59" s="20"/>
+      <c r="U59" s="20"/>
       <c r="AL59" s="12"/>
     </row>
     <row r="60" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Q60" s="9"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="20"/>
+      <c r="T60" s="20"/>
+      <c r="U60" s="20"/>
       <c r="AL60" s="12"/>
     </row>
     <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="20"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="20"/>
       <c r="AL61" s="12"/>
     </row>
     <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="20"/>
+      <c r="T62" s="20"/>
+      <c r="U62" s="20"/>
       <c r="AL62" s="12"/>
     </row>
     <row r="63" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-      <c r="M63" s="19"/>
+      <c r="Q63" s="20"/>
+      <c r="R63" s="20"/>
+      <c r="S63" s="20"/>
+      <c r="T63" s="20"/>
+      <c r="U63" s="20"/>
       <c r="AL63" s="12"/>
     </row>
     <row r="64" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="20"/>
-      <c r="M64" s="20"/>
+      <c r="Q64" s="9"/>
       <c r="AL64" s="12"/>
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="20"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65" s="20"/>
-      <c r="M65" s="20"/>
       <c r="AL65" s="12"/>
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL66" s="12"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
       <c r="AL67" s="12"/>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
       <c r="AL68" s="12"/>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="30"/>
       <c r="AL69" s="12"/>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
-      <c r="K70" s="12"/>
-      <c r="L70" s="12"/>
-      <c r="M70" s="12"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="12"/>
-      <c r="P70" s="12"/>
-      <c r="Q70" s="12"/>
-      <c r="R70" s="12"/>
-      <c r="S70" s="12"/>
-      <c r="T70" s="12"/>
-      <c r="U70" s="12"/>
-      <c r="V70" s="12"/>
-      <c r="W70" s="12"/>
-      <c r="X70" s="12"/>
-      <c r="Y70" s="12"/>
-      <c r="Z70" s="12"/>
-      <c r="AA70" s="12"/>
-      <c r="AB70" s="12"/>
-      <c r="AC70" s="12"/>
-      <c r="AD70" s="12"/>
-      <c r="AE70" s="12"/>
-      <c r="AF70" s="12"/>
-      <c r="AG70" s="12"/>
-      <c r="AH70" s="12"/>
-      <c r="AI70" s="12"/>
-      <c r="AJ70" s="12"/>
-      <c r="AK70" s="12"/>
       <c r="AL70" s="12"/>
     </row>
+    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL71" s="12"/>
+    </row>
+    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL72" s="12"/>
+    </row>
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL73" s="12"/>
+    </row>
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="12"/>
+      <c r="N74" s="12"/>
+      <c r="O74" s="12"/>
+      <c r="P74" s="12"/>
+      <c r="Q74" s="12"/>
+      <c r="R74" s="12"/>
+      <c r="S74" s="12"/>
+      <c r="T74" s="12"/>
+      <c r="U74" s="12"/>
+      <c r="V74" s="12"/>
+      <c r="W74" s="12"/>
+      <c r="X74" s="12"/>
+      <c r="Y74" s="12"/>
+      <c r="Z74" s="12"/>
+      <c r="AA74" s="12"/>
+      <c r="AB74" s="12"/>
+      <c r="AC74" s="12"/>
+      <c r="AD74" s="12"/>
+      <c r="AE74" s="12"/>
+      <c r="AF74" s="12"/>
+      <c r="AG74" s="12"/>
+      <c r="AH74" s="12"/>
+      <c r="AI74" s="12"/>
+      <c r="AJ74" s="12"/>
+      <c r="AK74" s="12"/>
+      <c r="AL74" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="38">
+    <mergeCell ref="B45:M47"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A67:M67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:M69"/>
+    <mergeCell ref="AD31:AJ33"/>
+    <mergeCell ref="AC31:AC33"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:M44"/>
+    <mergeCell ref="A42:M42"/>
+    <mergeCell ref="B52:F61"/>
+    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="Q55:U63"/>
+    <mergeCell ref="Q54:U54"/>
+    <mergeCell ref="O22:S44"/>
+    <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="W21:AA21"/>
+    <mergeCell ref="W22:AA41"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="I35:M35"/>
+    <mergeCell ref="J30:M31"/>
+    <mergeCell ref="I30:I31"/>
     <mergeCell ref="AO3:BD3"/>
     <mergeCell ref="AO23:BD23"/>
     <mergeCell ref="B3:F12"/>
@@ -4208,32 +4542,11 @@
     <mergeCell ref="O5:S15"/>
     <mergeCell ref="O4:S4"/>
     <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O22:S39"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:M17"/>
     <mergeCell ref="AD25:AJ25"/>
     <mergeCell ref="AD27:AJ28"/>
-    <mergeCell ref="AC27:AC28"/>
-    <mergeCell ref="W21:AA21"/>
-    <mergeCell ref="W22:AA41"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="I35:M35"/>
-    <mergeCell ref="J30:M31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A63:M63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:M65"/>
-    <mergeCell ref="AD31:AJ33"/>
-    <mergeCell ref="AC31:AC33"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:M44"/>
-    <mergeCell ref="A42:M42"/>
-    <mergeCell ref="B48:F57"/>
-    <mergeCell ref="A48:A57"/>
-    <mergeCell ref="Q51:U59"/>
-    <mergeCell ref="Q50:U50"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>